<commit_message>
[RM] practice on datasets for basic questions
</commit_message>
<xml_diff>
--- a/usingPandas/weather_data.xlsx
+++ b/usingPandas/weather_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmn7591/Documents/BITS/Practice/PFDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125E2EC7-7508-E149-9DCE-4FB3556886A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9E32B9-A0E5-1041-99C5-0E12EE757649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{2D856916-CC9D-154D-8F20-1AD52558EF4E}"/>
+    <workbookView xWindow="14900" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{2D856916-CC9D-154D-8F20-1AD52558EF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>day</t>
   </si>
@@ -47,9 +47,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>Nan</t>
-  </si>
-  <si>
     <t>Rain</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
   </si>
   <si>
     <t>Cloudy</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -427,7 +421,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,21 +451,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42767</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -481,25 +472,16 @@
       <c r="B4">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42826</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
       <c r="C5">
         <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -509,25 +491,13 @@
       <c r="B6">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42887</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -540,9 +510,6 @@
       <c r="C8">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -555,7 +522,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>